<commit_message>
Avance (Pasos finales del proyecto)
** Pedidos (solo usuario logeado)

-Formulario para realizar el pedido
-listado de pedidos(usuario)
-listado de todos los pedidos(admin)
-Modificar estatus del pedido (admin)
-viasualizar estatus del pedido (admin y user)

**Modifique el archivo que lleva el avance del proyecto (excel)
</commit_message>
<xml_diff>
--- a/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
+++ b/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\DW2\Armando Jovani Martinez Ruiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479AA3F0-A12E-4E37-BB95-BB725BA86493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F44500-D49C-417F-93CB-63386819E8AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -451,6 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,7 +475,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,62 +808,62 @@
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="11">
+      <c r="A4" s="20"/>
+      <c r="B4" s="10">
         <v>0.1</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>0.15</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>0.2</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>0.25</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>0.3</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>0.35</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>0.4</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>0.45</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>0.5</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <v>0.6</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="11">
         <v>0.65</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="11">
         <v>0.7</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="11">
         <v>0.75</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="11">
         <v>0.8</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="11">
         <v>0.85</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="11">
         <v>0.9</v>
       </c>
-      <c r="S4" s="12">
+      <c r="S4" s="11">
         <v>0.95</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -871,25 +871,25 @@
       <c r="A5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="8"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="7"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
@@ -897,12 +897,12 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -911,7 +911,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-      <c r="T6" s="9"/>
+      <c r="T6" s="8"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="32"/>
@@ -919,12 +919,12 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -933,61 +933,61 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-      <c r="T7" s="9"/>
+      <c r="T7" s="8"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="10"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="14"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1001,15 +1001,15 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="9"/>
+      <c r="T10" s="8"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1023,126 +1023,126 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="9"/>
+      <c r="T11" s="8"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="10"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="9"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="15"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="14"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
-      <c r="B14" s="27"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="9"/>
+      <c r="T14" s="8"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
-      <c r="B15" s="27"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="9"/>
+      <c r="T15" s="8"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="10"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="9"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1150,21 +1150,21 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="9"/>
+      <c r="T17" s="8"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1172,21 +1172,21 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="9"/>
+      <c r="T18" s="8"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1194,38 +1194,38 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="3"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="39"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="9"/>
+      <c r="T19" s="8"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="10"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Ultimos ajustes del proyecto y mejoras
**Productos

-  Búsqueda de productos

**Carrito de compras

- inormas al usuario el total a pagar de los productos del carrito

**Base de Datos

-Configuración para BD remota (heroku)

**Modifique el archivo excel que lleva el seguimiento del proyecto.
</commit_message>
<xml_diff>
--- a/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
+++ b/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\DW2\Armando Jovani Martinez Ruiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F44500-D49C-417F-93CB-63386819E8AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F805E-8579-4860-A39A-8166D5140460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,14 +413,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -433,7 +431,6 @@
     <xf numFmtId="9" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -451,6 +448,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -475,7 +473,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -761,7 +758,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,445 +784,445 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="38"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="10">
+      <c r="A4" s="17"/>
+      <c r="B4" s="8">
         <v>0.1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>0.15</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>0.2</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>0.25</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>0.3</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>0.35</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>0.4</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>0.45</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>0.5</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <v>0.6</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="9">
         <v>0.65</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>0.7</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="9">
         <v>0.75</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="9">
         <v>0.8</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="Q4" s="9">
         <v>0.85</v>
       </c>
-      <c r="R4" s="11">
+      <c r="R4" s="9">
         <v>0.9</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="9">
         <v>0.95</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="7"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="5"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="8"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="8"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="9"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="11"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="8"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="8"/>
+      <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="9"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="14"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="11"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="8"/>
+      <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="8"/>
+      <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="9"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="7"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="8"/>
+      <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="8"/>
+      <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="39"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="28"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="8"/>
+      <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="9"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Componentes extras (proyecto terminado)
**Productos (vista admin)

- Filtra los productos según la categoría para facilitar su gestión

** Pedidos (vista admin)

- Filtra los pedidos según el estatus del pedido (pendiente, en preparacion, empacado, enviado) para facilitar su visualización y gestión

**Documento excel

-Modifiqué la linea de avance del proyecto
</commit_message>
<xml_diff>
--- a/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
+++ b/Armando Jovani Martinez Ruiz/Avance proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\GitHub\DW2\Armando Jovani Martinez Ruiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430F805E-8579-4860-A39A-8166D5140460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF0B85D-69C1-4C9E-B509-0A70F800D5AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,9 +419,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,7 +428,6 @@
     <xf numFmtId="9" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -473,6 +469,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="T16" sqref="T13:T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,100 +784,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="36"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="8">
+      <c r="A4" s="13"/>
+      <c r="B4" s="5">
         <v>0.1</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>0.15</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>0.2</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>0.25</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>0.3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="6">
         <v>0.35</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>0.4</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="6">
         <v>0.45</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="6">
         <v>0.5</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="6">
         <v>0.6</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="6">
         <v>0.65</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="6">
         <v>0.7</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="6">
         <v>0.75</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="6">
         <v>0.8</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="6">
         <v>0.85</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="6">
         <v>0.9</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="6">
         <v>0.95</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -886,20 +886,20 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="5"/>
+      <c r="T5" s="36"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -908,20 +908,20 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="6"/>
+      <c r="T6" s="33"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -930,20 +930,20 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="6"/>
+      <c r="T7" s="33"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -952,35 +952,35 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="7"/>
+      <c r="T8" s="34"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="35"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -998,11 +998,11 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="6"/>
+      <c r="T10" s="33"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1020,15 +1020,15 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="6"/>
+      <c r="T11" s="33"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1042,35 +1042,35 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="7"/>
+      <c r="T12" s="34"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="11"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="35"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1088,11 +1088,11 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="6"/>
+      <c r="T14" s="33"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="23"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1110,35 +1110,35 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="6"/>
+      <c r="T15" s="33"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="7"/>
+      <c r="T16" s="34"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1156,11 +1156,11 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="6"/>
+      <c r="T17" s="33"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1178,11 +1178,11 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="6"/>
+      <c r="T18" s="33"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1195,23 +1195,23 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="28"/>
+      <c r="O19" s="24"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="6"/>
+      <c r="T19" s="33"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="16"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="27"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1222,7 +1222,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
-      <c r="T20" s="7"/>
+      <c r="T20" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>